<commit_message>
improve date handling and printing
</commit_message>
<xml_diff>
--- a/samples/sample1.xlsx
+++ b/samples/sample1.xlsx
@@ -33,10 +33,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="mmmm d, yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -48,12 +49,22 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -68,23 +79,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -108,23 +156,44 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -144,6 +213,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -1377,292 +1447,184 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I23"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.05469" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.05469" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.05469" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.05469" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.05469" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.05469" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.05469" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.05469" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.05469" style="1" customWidth="1"/>
-    <col min="10" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
+    <col min="10" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="19" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="D2" s="6">
+        <v>40831</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="9">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="9">
         <v>6</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="D3" s="10">
+        <v>40831.367870370370</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix worksheet reordering on save
</commit_message>
<xml_diff>
--- a/samples/sample1.xlsx
+++ b/samples/sample1.xlsx
@@ -6,13 +6,16 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="first" sheetId="1" r:id="rId4"/>
+    <sheet name="second" sheetId="2" r:id="rId5"/>
+    <sheet name="third" sheetId="3" r:id="rId6"/>
+    <sheet name="fourth" sheetId="4" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Table 1</t>
   </si>
@@ -27,6 +30,15 @@
   </si>
   <si>
     <t>string2</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>third</t>
+  </si>
+  <si>
+    <t>fourth</t>
   </si>
 </sst>
 </file>
@@ -70,7 +82,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +98,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -156,7 +180,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -194,6 +218,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -214,6 +259,8 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -1636,4 +1683,316 @@
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="13" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="13" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="13" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="13" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="B2" t="s" s="14">
+        <v>5</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="18" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="18" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="18" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="18" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="18" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="B2" t="s" s="14">
+        <v>6</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="19" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="19" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="19" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="19" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="19" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="B2" t="s" s="14">
+        <v>7</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>